<commit_message>
Split Book Distribution and Mentoring tabs, add BD Time Series chart and duplicate growth chart
</commit_message>
<xml_diff>
--- a/public/DashBoardData.xlsx
+++ b/public/DashBoardData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="60">
   <si>
     <t>Day</t>
   </si>
@@ -79,10 +79,16 @@
     <t>Points</t>
   </si>
   <si>
-    <t>Teja</t>
-  </si>
-  <si>
-    <t>Surakhshitha Devi</t>
+    <t>4 Jan</t>
+  </si>
+  <si>
+    <t>10 Jan</t>
+  </si>
+  <si>
+    <t>Teja Pr</t>
+  </si>
+  <si>
+    <t>Surakhshitha Mtj</t>
   </si>
   <si>
     <t>Kritesh pr</t>
@@ -151,34 +157,56 @@
     <t>Mentees</t>
   </si>
   <si>
-    <t>Kritesh Pr</t>
-  </si>
-  <si>
-    <t>Lokesh Pr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Teja Pr </t>
-  </si>
-  <si>
-    <t>Akash Pr</t>
-  </si>
-  <si>
-    <t>Teja Siva Pr</t>
+    <t xml:space="preserve">Naga Varun Pr &amp; Manisha Mtj </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lokesh Pr &amp; Kavya Mtj </t>
+  </si>
+  <si>
+    <t>Teja Pr &amp; Surakhshitha Mtj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siva Sagar Pr &amp; Anusha S Mtj </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brahmaleela Mtj </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sreenivas Pr &amp; Vishnu Priyanka Mtj </t>
+  </si>
+  <si>
+    <t>Sai Varun Pr</t>
   </si>
   <si>
     <t>Worksheets</t>
   </si>
   <si>
-    <t xml:space="preserve">A+ / A </t>
+    <t>28th Dec</t>
+  </si>
+  <si>
+    <t>4th Jan</t>
+  </si>
+  <si>
+    <t>11th Jan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18th Jan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">25th Jan </t>
+  </si>
+  <si>
+    <t>1st Feb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="mmm-d"/>
     <numFmt numFmtId="165" formatCode="mmm - d"/>
+    <numFmt numFmtId="166" formatCode="d mmm"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -235,6 +263,34 @@
     <border/>
     <border>
       <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF284E3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF6F8F9"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF284E3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF6F8F9"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFF6F8F9"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF284E3F"/>
       </left>
       <right style="thin">
@@ -249,38 +305,10 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF284E3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF284E3F"/>
       </left>
       <right style="thin">
         <color rgb="FFF6F8F9"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFF6F8F9"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFF6F8F9"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFF6F8F9"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF284E3F"/>
       </right>
       <top style="thin">
         <color rgb="FFF6F8F9"/>
@@ -321,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -345,20 +373,30 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="right" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="right" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="3" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="2" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="4" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="4" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" wrapText="0"/>
+    <xf borderId="3" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="5" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="0"/>
     </xf>
@@ -651,7 +689,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="6.0"/>
+    <col customWidth="1" min="1" max="1" width="7.25"/>
     <col customWidth="1" min="2" max="2" width="10.13"/>
     <col customWidth="1" min="3" max="3" width="15.13"/>
     <col customWidth="1" min="4" max="4" width="11.75"/>
@@ -793,6 +831,26 @@
         <v>9.0</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" s="5">
+        <v>46068.0</v>
+      </c>
+      <c r="B8" s="4">
+        <v>56.0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>27.0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>30.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5"/>
+      <c r="B9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1097,6 +1155,26 @@
         <v>15</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" s="3">
+        <v>46068.0</v>
+      </c>
+      <c r="B8" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>14.0</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1116,6 +1194,11 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="15.63"/>
+    <col customWidth="1" min="4" max="4" width="14.5"/>
+    <col customWidth="1" min="5" max="5" width="7.88"/>
+    <col customWidth="1" min="6" max="6" width="8.75"/>
+    <col customWidth="1" min="9" max="10" width="6.63"/>
+    <col customWidth="1" min="11" max="11" width="7.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1125,181 +1208,397 @@
       <c r="B1" s="8" t="s">
         <v>19</v>
       </c>
+      <c r="D1" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="10">
+        <v>46039.0</v>
+      </c>
+      <c r="H1" s="10">
+        <v>46047.0</v>
+      </c>
+      <c r="I1" s="10">
+        <v>46054.0</v>
+      </c>
+      <c r="J1" s="10">
+        <v>46060.0</v>
+      </c>
+      <c r="K1" s="10">
+        <v>46067.0</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="10">
-        <v>146.33333333333334</v>
+      <c r="A2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="11">
+        <v>194.33333333333331</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="6">
+        <v>19.0</v>
+      </c>
+      <c r="F2" s="6">
+        <v>36.5</v>
+      </c>
+      <c r="G2" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="H2" s="6">
+        <v>35.5</v>
+      </c>
+      <c r="I2" s="6">
+        <v>4.5</v>
+      </c>
+      <c r="J2" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="K2" s="6">
+        <v>18.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="11" t="s">
-        <v>21</v>
+      <c r="A3" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="B3" s="12">
-        <v>99.5</v>
+        <v>135.0</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="6">
+        <v>31.5</v>
+      </c>
+      <c r="G3" s="6">
+        <v>17.0</v>
+      </c>
+      <c r="H3" s="6">
+        <v>15.5</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="K3" s="6">
+        <v>18.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="10">
-        <v>157.58333333333334</v>
+      <c r="A4" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="11">
+        <v>244.08333333333334</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="6">
+        <v>51.5</v>
+      </c>
+      <c r="F4" s="6">
+        <v>14.0</v>
+      </c>
+      <c r="G4" s="14">
+        <v>26.166666666666668</v>
+      </c>
+      <c r="H4" s="14">
+        <v>27.5</v>
+      </c>
+      <c r="I4" s="14">
+        <v>17.666666666666668</v>
+      </c>
+      <c r="J4" s="14">
+        <v>18.0</v>
+      </c>
+      <c r="K4" s="14">
+        <v>36.5</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="11" t="s">
-        <v>23</v>
+      <c r="A5" s="15" t="s">
+        <v>25</v>
       </c>
       <c r="B5" s="12">
-        <v>50.083333333333336</v>
+        <v>75.5</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="6">
+        <v>8.0</v>
+      </c>
+      <c r="F5" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="H5" s="6">
+        <v>10.5</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="J5" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="10">
+      <c r="A6" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="11">
         <v>16.0</v>
       </c>
+      <c r="D6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="11" t="s">
-        <v>25</v>
+      <c r="A7" s="15" t="s">
+        <v>27</v>
       </c>
       <c r="B7" s="12">
-        <v>100.75</v>
+        <v>141.33333333333334</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="6">
+        <v>51.5</v>
+      </c>
+      <c r="F7" s="6">
+        <v>9.0</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="I7" s="6">
+        <v>10.0</v>
+      </c>
+      <c r="J7" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="K7" s="6">
+        <v>18.5</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="10">
-        <v>140.0</v>
+      <c r="A8" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="11">
+        <v>179.58333333333334</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="F8" s="6">
+        <v>19.0</v>
+      </c>
+      <c r="G8" s="14">
+        <v>4.666666666666667</v>
+      </c>
+      <c r="H8" s="14">
+        <v>15.5</v>
+      </c>
+      <c r="I8" s="14">
+        <v>10.0</v>
+      </c>
+      <c r="J8" s="14">
+        <v>8.5</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="11" t="s">
-        <v>27</v>
+      <c r="A9" s="15" t="s">
+        <v>29</v>
       </c>
       <c r="B9" s="12">
-        <v>196.83333333333331</v>
+        <v>228.08333333333331</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="F9" s="6">
+        <v>19.0</v>
+      </c>
+      <c r="G9" s="6">
+        <v>11.0</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="J9" s="6">
+        <v>8.5</v>
+      </c>
+      <c r="K9" s="6">
+        <v>0.0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="13">
-        <v>36.5</v>
+      <c r="A10" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="17">
+        <v>41.5</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="14">
-        <v>36.5</v>
+      <c r="A11" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="18">
+        <v>41.5</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="13">
-        <v>42.5</v>
+      <c r="A12" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="17">
+        <v>43.33333333333333</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="14">
-        <v>49.0</v>
+      <c r="A13" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="18">
+        <v>52.33333333333333</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="13">
-        <v>28.5</v>
+      <c r="A14" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="17">
+        <v>39.166666666666664</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="14">
-        <v>8.5</v>
+      <c r="A15" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="18">
+        <v>11.0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="13">
-        <v>31.5</v>
+      <c r="A16" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="17">
+        <v>32.33333333333333</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="14">
-        <v>31.5</v>
+      <c r="A17" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="18">
+        <v>32.33333333333333</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="13">
-        <v>28.5</v>
+      <c r="A18" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="17">
+        <v>32.25</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="14">
-        <v>18.5</v>
+      <c r="A19" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="18">
+        <v>21.0</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="13">
-        <v>0.0</v>
+      <c r="A20" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="17">
+        <v>4.0</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="14">
-        <v>15.0</v>
+      <c r="A21" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="18">
+        <v>17.5</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="13">
-        <v>21.75</v>
+      <c r="A22" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="17">
+        <v>29.666666666666668</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="16">
-        <v>32.5</v>
+      <c r="A23" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="20">
+        <v>37.5</v>
       </c>
     </row>
   </sheetData>
@@ -1319,18 +1618,21 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="29.38"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B2" s="4">
         <v>5.0</v>
@@ -1340,28 +1642,28 @@
       </c>
       <c r="E2" s="6">
         <f>SUM(B:B)</f>
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B3" s="4">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B4" s="4">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B5" s="4">
         <v>4.0</v>
@@ -1369,10 +1671,26 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B6" s="4">
-        <v>5.0</v>
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="4">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="4">
+        <v>2.0</v>
       </c>
     </row>
   </sheetData>
@@ -1395,48 +1713,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4">
-        <v>1.0</v>
+      <c r="A2" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="B2" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" s="4">
-        <v>26.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4">
-        <v>2.0</v>
+      <c r="A3" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="B3" s="4">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="4">
         <v>3.0</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="B4" s="4">
-        <v>2.0</v>
-      </c>
-    </row>
     <row r="5">
-      <c r="A5" s="4">
+      <c r="A5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="4">
         <v>4.0</v>
       </c>
-      <c r="B5" s="4">
-        <v>1.0</v>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="4">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="4">
+        <v>6.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>